<commit_message>
Changes from the meeting
</commit_message>
<xml_diff>
--- a/Communication/priority_proposal.xlsx
+++ b/Communication/priority_proposal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niklasthurnau/Desktop/Uni/PRJ3_2/prj3-2020-traffic-control-international-prj3-2020-group-05/Communication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3E7572-B769-2246-B723-E15EEBE05326}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DB308E-2B00-4840-8A0C-92B8BCBAA1ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="17100" xr2:uid="{8B7F7293-A4EB-4E4F-BD89-75F4F3B15E3E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>SRS</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>UI</t>
+  </si>
+  <si>
+    <t>Very High</t>
   </si>
 </sst>
 </file>
@@ -447,7 +450,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -472,7 +475,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -512,7 +515,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -528,7 +531,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -581,8 +584,8 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B14" xr:uid="{823722CB-2269-9645-9DE0-378DDF242204}">
-      <formula1>"High,Medium,Low"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B15" xr:uid="{84FA943A-4E2B-7743-9809-C169D99FD10E}">
+      <formula1>"Very High, High, Medium, Low,"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>